<commit_message>
updated excel file - updated query and result for Q3
</commit_message>
<xml_diff>
--- a/answers.xlsx
+++ b/answers.xlsx
@@ -2725,44 +2725,44 @@
   <si>
     <t>select DISTINCT VendorName
 from 
-	(select VendorName, sum(AmountGross) as total 
-	from expenses
-	where EmployeeName &lt;&gt; VendorName and VendorName = upper(VendorName) and Quarter = 2
-	group by VendorName)
+        (select VendorName, sum(AmountGross) as total 
+        from expenses
+        where EmployeeName &lt;&gt; VendorName and VendorName = upper(VendorName) and Quarter = 2 and ExpenseCategory LIKE '%Meals%'
+        group by VendorName)
 order by total desc limit 10</t>
   </si>
   <si>
     <t>VendorName</t>
   </si>
   <si>
-    <t>OTTER TAIL CORPORATION</t>
-  </si>
-  <si>
     <t>THUMPER POND G C</t>
   </si>
   <si>
-    <t>OTTER TAIL POWER COMPANY</t>
-  </si>
-  <si>
-    <t>BEST WESTERN HOTEL</t>
+    <t>ANNUAL SHAREHOLDER MEETING</t>
+  </si>
+  <si>
+    <t>ZENS CREATIVE CATERING</t>
+  </si>
+  <si>
+    <t>LEAN MASTERY TRAINING</t>
+  </si>
+  <si>
+    <t>BIG STONE POWER PLANT</t>
+  </si>
+  <si>
+    <t>VIKING CAFE</t>
+  </si>
+  <si>
+    <t>PIONEERCARE</t>
+  </si>
+  <si>
+    <t>VETERANS CLUB</t>
   </si>
   <si>
     <t>CHIEFTAIN CONFERENCE C</t>
   </si>
   <si>
-    <t>ANNUAL SHAREHOLDER MEETING</t>
-  </si>
-  <si>
     <t>RAMADA PLAZA SUITES</t>
-  </si>
-  <si>
-    <t>BIG STONE POWER PLANT</t>
-  </si>
-  <si>
-    <t>BEST WESTERN KELLY INN</t>
-  </si>
-  <si>
-    <t>BECKLUND OIL INC</t>
   </si>
   <si>
     <t>select DayName, count(*) as number, sum(AmountGross) as amount

</xml_diff>